<commit_message>
Deployed 2b71b7c1 with MkDocs version: 1.5.3
</commit_message>
<xml_diff>
--- a/general/BS Virtualisierungsprojekt.xlsx
+++ b/general/BS Virtualisierungsprojekt.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t xml:space="preserve">Datum</t>
   </si>
@@ -67,43 +67,55 @@
     <t xml:space="preserve">19.2.2024</t>
   </si>
   <si>
+    <t xml:space="preserve">Trace-cmd und KernelShark funktionieren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.2.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isolate CPUs of Host</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.3.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decrease latency </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.3.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preempt_RT Kernel Patch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.3.2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">Zeitmessungen und Vergleiche zwischen verschiedenen Virtualisierungsmöglichkeiten unter Ubuntu sollen abgeschlossen sein</t>
   </si>
   <si>
-    <t xml:space="preserve">26.2.2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.3.2024</t>
+    <t xml:space="preserve">25.3.2024</t>
   </si>
   <si>
     <t xml:space="preserve">QEMU/WSL unter Windows lauffähig</t>
   </si>
   <si>
-    <t xml:space="preserve">11.3.2024</t>
+    <t xml:space="preserve">1.4.2024</t>
   </si>
   <si>
     <t xml:space="preserve">Zeitmessungen und Vergleiche zwischen verschiedenen Virualisierungsmöglichkeiten unter Windows sollen abgeschlossen sein</t>
   </si>
   <si>
-    <t xml:space="preserve">18.3.2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25.3.2024</t>
+    <t xml:space="preserve">8.4.2024</t>
   </si>
   <si>
     <t xml:space="preserve">Zeitmessungen abgeschlossen Konklusio und Aufarbeitung/Vergleich PreemptRT gegen Xenomai</t>
   </si>
   <si>
-    <t xml:space="preserve">1.4.2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.4.2024</t>
+    <t xml:space="preserve">15.4.2024</t>
   </si>
   <si>
     <t xml:space="preserve">Dedizierte Ressourcenzuteilung unter Windows und Messung Verhalten (Core-Sperrung,…)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15.4.2024</t>
   </si>
   <si>
     <t xml:space="preserve">22.4.2024</t>
@@ -231,7 +243,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -261,6 +273,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -348,10 +364,10 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="11.86"/>
@@ -453,146 +469,157 @@
         <v>9</v>
       </c>
       <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
+      <c r="D8" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>17</v>
+      <c r="A9" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="B9" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4" t="s">
-        <v>18</v>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
-        <v>19</v>
+      <c r="A10" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="B10" s="8" t="n">
         <v>11</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4" t="s">
-        <v>20</v>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="8" t="n">
+        <v>22</v>
+      </c>
+      <c r="B11" s="9" t="n">
         <v>12</v>
       </c>
       <c r="C11" s="4"/>
+      <c r="D11" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="8" t="n">
+        <v>24</v>
+      </c>
+      <c r="B12" s="9" t="n">
         <v>13</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="8" t="n">
+        <v>26</v>
+      </c>
+      <c r="B13" s="9" t="n">
         <v>14</v>
       </c>
       <c r="C13" s="4"/>
+      <c r="D13" s="4" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="8" t="n">
+        <v>28</v>
+      </c>
+      <c r="B14" s="9" t="n">
         <v>15</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="8" t="n">
+        <v>30</v>
+      </c>
+      <c r="B15" s="9" t="n">
         <v>16</v>
       </c>
       <c r="C15" s="4"/>
+      <c r="D15" s="4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="8" t="n">
+        <v>32</v>
+      </c>
+      <c r="B16" s="9" t="n">
         <v>17</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="8" t="n">
+        <v>34</v>
+      </c>
+      <c r="B17" s="9" t="n">
         <v>18</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="8" t="n">
+        <v>36</v>
+      </c>
+      <c r="B18" s="9" t="n">
         <v>19</v>
       </c>
       <c r="C18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="8" t="n">
+        <v>37</v>
+      </c>
+      <c r="B19" s="9" t="n">
         <v>20</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="8" t="n">
+        <v>39</v>
+      </c>
+      <c r="B20" s="9" t="n">
         <v>21</v>
       </c>
       <c r="C20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="8" t="n">
+        <v>40</v>
+      </c>
+      <c r="B21" s="9" t="n">
         <v>22</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deployed 0405cc4 with MkDocs version: 1.6.0
</commit_message>
<xml_diff>
--- a/general/BS Virtualisierungsprojekt.xlsx
+++ b/general/BS Virtualisierungsprojekt.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t xml:space="preserve">Datum</t>
   </si>
@@ -91,61 +91,52 @@
     <t xml:space="preserve">18.3.2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Zeitmessungen und Vergleiche zwischen verschiedenen Virtualisierungsmöglichkeiten unter Ubuntu sollen abgeschlossen sein</t>
-  </si>
-  <si>
     <t xml:space="preserve">25.3.2024</t>
   </si>
   <si>
-    <t xml:space="preserve">QEMU/WSL unter Windows lauffähig</t>
-  </si>
-  <si>
     <t xml:space="preserve">1.4.2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Zeitmessungen und Vergleiche zwischen verschiedenen Virualisierungsmöglichkeiten unter Windows sollen abgeschlossen sein</t>
-  </si>
-  <si>
     <t xml:space="preserve">8.4.2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Zeitmessungen abgeschlossen Konklusio und Aufarbeitung/Vergleich PreemptRT gegen Xenomai</t>
-  </si>
-  <si>
     <t xml:space="preserve">15.4.2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Dedizierte Ressourcenzuteilung unter Windows und Messung Verhalten (Core-Sperrung,…)</t>
-  </si>
-  <si>
     <t xml:space="preserve">22.4.2024</t>
   </si>
   <si>
+    <t xml:space="preserve">29.4.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ubuntu real-time kernel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.5.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.5.2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reduced latency in QEMU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.5.2026</t>
+  </si>
+  <si>
     <t xml:space="preserve">VARAN Einsteckkarte lauffähig</t>
   </si>
   <si>
-    <t xml:space="preserve">29.4.2024</t>
+    <t xml:space="preserve">27.5.2027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abgabe Masterarbeit</t>
   </si>
   <si>
     <t xml:space="preserve">VARAN Zeitmessungen abgeschlossen</t>
   </si>
   <si>
-    <t xml:space="preserve">6.5.2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.5.2025</t>
-  </si>
-  <si>
     <t xml:space="preserve">LasalClass2 Applikation für Robotersteuerung lauffähig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20.5.2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27.5.2027</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abgabe Masterarbeit</t>
   </si>
 </sst>
 </file>
@@ -243,7 +234,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -278,6 +269,18 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -361,13 +364,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="11.86"/>
@@ -498,129 +501,135 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="9" t="n">
+      <c r="B11" s="10" t="n">
         <v>12</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4" t="s">
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
+      <c r="B12" s="10" t="n">
+        <v>13</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="9" t="n">
-        <v>13</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4" t="s">
+      <c r="B13" s="10" t="n">
+        <v>14</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="9" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
+      <c r="B14" s="10" t="n">
+        <v>15</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="9" t="n">
-        <v>14</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4" t="s">
+      <c r="B15" s="10" t="n">
+        <v>16</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="11"/>
+    </row>
+    <row r="16" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
+      <c r="B16" s="10" t="n">
+        <v>17</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="11"/>
+    </row>
+    <row r="17" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="9" t="n">
-        <v>15</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4" t="s">
+      <c r="B17" s="10" t="n">
+        <v>18</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
+    <row r="18" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="9" t="n">
-        <v>16</v>
-      </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4" t="s">
+      <c r="B18" s="10" t="n">
+        <v>19</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="11"/>
+    </row>
+    <row r="19" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="9" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
+      <c r="B19" s="10" t="n">
+        <v>20</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="11" t="s">
         <v>32</v>
-      </c>
-      <c r="B16" s="9" t="n">
-        <v>17</v>
-      </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="9" t="n">
-        <v>18</v>
-      </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="9" t="n">
-        <v>19</v>
-      </c>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="9" t="n">
-        <v>20</v>
-      </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="9" t="n">
+        <v>33</v>
+      </c>
+      <c r="B20" s="12" t="n">
         <v>21</v>
       </c>
       <c r="C20" s="4"/>
+      <c r="D20" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="9" t="n">
+        <v>35</v>
+      </c>
+      <c r="B21" s="12" t="n">
         <v>22</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>41</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D22" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D23" s="0"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D24" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Deployed f49667b with MkDocs version: 1.6.0
</commit_message>
<xml_diff>
--- a/general/BS Virtualisierungsprojekt.xlsx
+++ b/general/BS Virtualisierungsprojekt.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t xml:space="preserve">Datum</t>
   </si>
@@ -124,13 +124,16 @@
     <t xml:space="preserve">20.5.2026</t>
   </si>
   <si>
+    <t xml:space="preserve">Reduced latency even more</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.5.2027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abgabe Masterarbeit</t>
+  </si>
+  <si>
     <t xml:space="preserve">VARAN Einsteckkarte lauffähig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27.5.2027</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abgabe Masterarbeit</t>
   </si>
   <si>
     <t xml:space="preserve">VARAN Zeitmessungen abgeschlossen</t>
@@ -147,7 +150,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -169,6 +172,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -234,7 +243,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -285,6 +294,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -364,13 +377,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="11.86"/>
@@ -602,7 +615,7 @@
         <v>21</v>
       </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="13" t="s">
         <v>34</v>
       </c>
     </row>
@@ -616,20 +629,25 @@
       <c r="C21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="0"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D22" s="0"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D23" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D22" s="4" t="s">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D24" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D23" s="0"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D24" s="0"/>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D25" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>